<commit_message>
Added structural coverage: 42.2%
</commit_message>
<xml_diff>
--- a/Refinements.xlsx
+++ b/Refinements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrtollefson/Desktop/VisionInfo/vision_structures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F35C543-24C3-464E-896D-3D5E9BF6BEEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A42B629-951B-BB43-B937-24F923F8FD2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{7FC0642B-9DD0-8545-8874-DC3822DB7C02}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19400" xr2:uid="{7FC0642B-9DD0-8545-8874-DC3822DB7C02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{E7EF7BB9-F9B8-2840-8F07-D617B53611D7}" name="newDat" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/mrtollefson/Desktop/VisionInfo/vision_structures/newDat.csv" comma="1">
+    <textPr sourceFile="/Users/mrtollefson/Desktop/VisionInfo/vision_structures/newDat.csv" comma="1">
       <textFields count="17">
         <textField/>
         <textField/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="403">
   <si>
     <t>ABCA4</t>
   </si>
@@ -1262,6 +1262,9 @@
   </si>
   <si>
     <t>PEX6-Hexamer(*used monomer)</t>
+  </si>
+  <si>
+    <t>Vision Coverage</t>
   </si>
 </sst>
 </file>
@@ -1293,7 +1296,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1325,15 +1328,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1652,11 +1687,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296894DF-B6BA-6A4E-921F-FBE76FD48E42}">
-  <dimension ref="A1:Q279"/>
+  <dimension ref="A1:Q284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A187" sqref="A187"/>
+      <pane ySplit="1" topLeftCell="A262" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F289" sqref="F289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14892,56 +14927,68 @@
         <v>438.60377358490564</v>
       </c>
       <c r="E279" s="1">
-        <f>AVERAGE(E2:E278)</f>
+        <f t="shared" ref="E279:Q279" si="0">AVERAGE(E2:E278)</f>
         <v>1029.4392523364486</v>
       </c>
       <c r="F279" s="1">
-        <f>AVERAGE(F2:F278)</f>
+        <f t="shared" si="0"/>
         <v>33.995342960288816</v>
       </c>
       <c r="G279" s="1">
-        <f>AVERAGE(G2:G278)</f>
+        <f t="shared" si="0"/>
         <v>33.345794392523359</v>
       </c>
       <c r="H279" s="1">
-        <f>AVERAGE(H2:H278)</f>
+        <f t="shared" si="0"/>
         <v>2.2351985559566776</v>
       </c>
       <c r="I279" s="1">
-        <f>AVERAGE(I2:I278)</f>
+        <f t="shared" si="0"/>
         <v>29.317689530685918</v>
       </c>
       <c r="J279" s="1">
-        <f>AVERAGE(J2:J278)</f>
+        <f t="shared" si="0"/>
         <v>2.2669314079422391</v>
       </c>
       <c r="K279" s="1">
-        <f>AVERAGE(K2:K278)</f>
+        <f t="shared" si="0"/>
         <v>91.48234657039707</v>
       </c>
       <c r="L279" s="1">
-        <f>AVERAGE(L2:L278)</f>
+        <f t="shared" si="0"/>
         <v>2.2323104693140796</v>
       </c>
       <c r="M279" s="1">
-        <f>AVERAGE(M2:M278)</f>
+        <f t="shared" si="0"/>
         <v>1.7940433212996392</v>
       </c>
       <c r="N279" s="1">
-        <f>AVERAGE(N2:N278)</f>
+        <f t="shared" si="0"/>
         <v>0.42657039711191336</v>
       </c>
       <c r="O279" s="1">
-        <f>AVERAGE(O2:O278)</f>
+        <f t="shared" si="0"/>
         <v>1.1675812274368231</v>
       </c>
       <c r="P279" s="1">
-        <f>AVERAGE(P2:P278)</f>
+        <f t="shared" si="0"/>
         <v>92.598231046931389</v>
       </c>
       <c r="Q279" s="1">
-        <f>AVERAGE(Q2:Q278)</f>
+        <f t="shared" si="0"/>
         <v>1.1071119133574008</v>
+      </c>
+    </row>
+    <row r="282" spans="1:17" ht="17" thickBot="1"/>
+    <row r="283" spans="1:17">
+      <c r="D283" s="4" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="284" spans="1:17" ht="17" thickBot="1">
+      <c r="D284" s="5">
+        <f>(SUM(D2:D278))/(SUM(E2:E278))</f>
+        <v>0.42207898320472081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>